<commit_message>
add car type prediction
</commit_message>
<xml_diff>
--- a/data/fuel-consumption.xlsx
+++ b/data/fuel-consumption.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Python Scripts\AI\UTS\fuel-efficiency-prediction\project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7609AD-B257-4065-B799-584D6A17C2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D45914-0AF3-4DF8-BBA3-7CC0B1D175CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CF2E0BD1-D766-41EB-86A8-26B2C2952F93}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="180">
   <si>
     <t>car name</t>
   </si>
@@ -183,9 +183,6 @@
     <t>maxda glc deluxe</t>
   </si>
   <si>
-    <t>dodge colt hatchback custom</t>
-  </si>
-  <si>
     <t>amc spirit dl</t>
   </si>
   <si>
@@ -252,9 +249,6 @@
     <t>mazda 626</t>
   </si>
   <si>
-    <t>datsun 510 hatchback</t>
-  </si>
-  <si>
     <t>toyota corolla</t>
   </si>
   <si>
@@ -309,9 +303,6 @@
     <t>buick skylark</t>
   </si>
   <si>
-    <t>dodge aries wagon (sw)</t>
-  </si>
-  <si>
     <t>toyota starlet</t>
   </si>
   <si>
@@ -321,9 +312,6 @@
     <t>honda civic 1300</t>
   </si>
   <si>
-    <t>subaru</t>
-  </si>
-  <si>
     <t>datsun 210 mpg</t>
   </si>
   <si>
@@ -381,15 +369,9 @@
     <t>chevrolet cavalier</t>
   </si>
   <si>
-    <t>chevrolet cavalier wagon</t>
-  </si>
-  <si>
     <t>chevrolet cavalier 2-door</t>
   </si>
   <si>
-    <t>pontiac j2000 se hatchback</t>
-  </si>
-  <si>
     <t>dodge aries se</t>
   </si>
   <si>
@@ -450,9 +432,6 @@
     <t>ford mustang gl</t>
   </si>
   <si>
-    <t>vw pickup</t>
-  </si>
-  <si>
     <t>dodge rampage</t>
   </si>
   <si>
@@ -577,6 +556,27 @@
   </si>
   <si>
     <t>82</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>dodge colt 3</t>
+  </si>
+  <si>
+    <t>datsun 510 3</t>
+  </si>
+  <si>
+    <t>pontiac j2000 se 3</t>
+  </si>
+  <si>
+    <t>dodge aries 6 (sw)</t>
+  </si>
+  <si>
+    <t>chevrolet cavalier 6</t>
+  </si>
+  <si>
+    <t>vw 7</t>
   </si>
 </sst>
 </file>
@@ -968,11 +968,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CC87CE-3523-402F-9F52-FD64AB22A2C5}">
-  <dimension ref="A1:G143"/>
+  <dimension ref="A1:H142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,9 +983,10 @@
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1005,10 +1006,13 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1028,10 +1032,13 @@
         <v>22</v>
       </c>
       <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
         <v>12.04</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1051,10 +1058,13 @@
         <v>22</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>14.6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1074,10 +1084,13 @@
         <v>20</v>
       </c>
       <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>11.8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1097,10 +1110,13 @@
         <v>21</v>
       </c>
       <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
         <v>11.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1120,10 +1136,13 @@
         <v>20</v>
       </c>
       <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1143,10 +1162,13 @@
         <v>21</v>
       </c>
       <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
         <v>18.41</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -1166,10 +1188,13 @@
         <v>22</v>
       </c>
       <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
         <v>14.1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
@@ -1189,10 +1214,13 @@
         <v>21</v>
       </c>
       <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
         <v>10.9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -1212,10 +1240,13 @@
         <v>17</v>
       </c>
       <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
         <v>12.8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
@@ -1235,10 +1266,13 @@
         <v>22</v>
       </c>
       <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <v>12.4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -1258,10 +1292,13 @@
         <v>15</v>
       </c>
       <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
         <v>11.2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1275,16 +1312,19 @@
         <v>107</v>
       </c>
       <c r="E13" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F13">
         <v>15</v>
       </c>
       <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>11.3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
@@ -1304,10 +1344,13 @@
         <v>22</v>
       </c>
       <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
         <v>14.9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1327,10 +1370,13 @@
         <v>15</v>
       </c>
       <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
@@ -1350,10 +1396,13 @@
         <v>12</v>
       </c>
       <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
         <v>11.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
@@ -1373,10 +1422,13 @@
         <v>17</v>
       </c>
       <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
@@ -1396,10 +1448,13 @@
         <v>20</v>
       </c>
       <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
         <v>12.2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
@@ -1419,10 +1474,13 @@
         <v>15</v>
       </c>
       <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
         <v>16.2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1442,10 +1500,13 @@
         <v>14</v>
       </c>
       <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20">
         <v>12.2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
@@ -1459,16 +1520,19 @@
         <v>118</v>
       </c>
       <c r="E21" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F21">
         <v>17</v>
       </c>
       <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
         <v>12.7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
@@ -1488,10 +1552,13 @@
         <v>13</v>
       </c>
       <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
         <v>13.2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
@@ -1511,10 +1578,13 @@
         <v>4</v>
       </c>
       <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
         <v>11.4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>28</v>
       </c>
@@ -1534,10 +1604,13 @@
         <v>17</v>
       </c>
       <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
         <v>11.2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>29</v>
       </c>
@@ -1557,10 +1630,13 @@
         <v>0</v>
       </c>
       <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>30</v>
       </c>
@@ -1580,10 +1656,13 @@
         <v>19</v>
       </c>
       <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
         <v>9.4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
@@ -1597,16 +1676,19 @@
         <v>140</v>
       </c>
       <c r="E27" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F27">
         <v>19</v>
       </c>
       <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>32</v>
       </c>
@@ -1626,10 +1708,13 @@
         <v>15</v>
       </c>
       <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -1649,10 +1734,13 @@
         <v>20</v>
       </c>
       <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
         <v>13.5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>44</v>
       </c>
@@ -1672,10 +1760,13 @@
         <v>18</v>
       </c>
       <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>36</v>
       </c>
@@ -1695,10 +1786,13 @@
         <v>18</v>
       </c>
       <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>37</v>
       </c>
@@ -1718,10 +1812,13 @@
         <v>18</v>
       </c>
       <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="H32">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>38</v>
       </c>
@@ -1741,10 +1838,13 @@
         <v>18</v>
       </c>
       <c r="G33">
+        <v>4</v>
+      </c>
+      <c r="H33">
         <v>7.3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>39</v>
       </c>
@@ -1764,10 +1864,13 @@
         <v>18</v>
       </c>
       <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>40</v>
       </c>
@@ -1787,10 +1890,13 @@
         <v>18</v>
       </c>
       <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
         <v>11.6</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>41</v>
       </c>
@@ -1810,10 +1916,13 @@
         <v>18</v>
       </c>
       <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>42</v>
       </c>
@@ -1833,10 +1942,13 @@
         <v>18</v>
       </c>
       <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
         <v>11.9</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>43</v>
       </c>
@@ -1856,10 +1968,13 @@
         <v>18</v>
       </c>
       <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
         <v>21.7</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1879,10 +1994,13 @@
         <v>70</v>
       </c>
       <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>46</v>
       </c>
@@ -1902,10 +2020,13 @@
         <v>70</v>
       </c>
       <c r="G40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -1916,7 +2037,7 @@
         <v>1409</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E41">
         <v>1975</v>
@@ -1925,12 +2046,15 @@
         <v>79</v>
       </c>
       <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -1939,7 +2063,7 @@
         <v>1605</v>
       </c>
       <c r="D42" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E42">
         <v>1915</v>
@@ -1948,12 +2072,15 @@
         <v>79</v>
       </c>
       <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
         <v>15.1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -1962,7 +2089,7 @@
         <v>1982</v>
       </c>
       <c r="D43" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E43">
         <v>2670</v>
@@ -1971,12 +2098,15 @@
         <v>79</v>
       </c>
       <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
         <v>11.6</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B44">
         <v>5</v>
@@ -1985,7 +2115,7 @@
         <v>2998</v>
       </c>
       <c r="D44" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E44">
         <v>3530</v>
@@ -1994,12 +2124,15 @@
         <v>79</v>
       </c>
       <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44">
         <v>10.7</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45">
         <v>8</v>
@@ -2008,7 +2141,7 @@
         <v>5735</v>
       </c>
       <c r="D45" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E45">
         <v>3900</v>
@@ -2017,12 +2150,15 @@
         <v>79</v>
       </c>
       <c r="G45">
+        <v>4</v>
+      </c>
+      <c r="H45">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -2031,7 +2167,7 @@
         <v>2310</v>
       </c>
       <c r="D46" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E46">
         <v>3190</v>
@@ -2040,12 +2176,15 @@
         <v>79</v>
       </c>
       <c r="G46">
+        <v>4</v>
+      </c>
+      <c r="H46">
         <v>11.5</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -2054,7 +2193,7 @@
         <v>1720</v>
       </c>
       <c r="D47" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E47">
         <v>2200</v>
@@ -2063,12 +2202,15 @@
         <v>79</v>
       </c>
       <c r="G47">
+        <v>3</v>
+      </c>
+      <c r="H47">
         <v>14.5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48">
         <v>4</v>
@@ -2077,7 +2219,7 @@
         <v>1720</v>
       </c>
       <c r="D48" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E48">
         <v>2150</v>
@@ -2086,12 +2228,15 @@
         <v>79</v>
       </c>
       <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="H48">
         <v>14.6</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B49">
         <v>4</v>
@@ -2100,7 +2245,7 @@
         <v>1392</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E49">
         <v>2020</v>
@@ -2109,12 +2254,15 @@
         <v>79</v>
       </c>
       <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49">
         <v>13.5</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50">
         <v>4</v>
@@ -2123,7 +2271,7 @@
         <v>1491</v>
       </c>
       <c r="D50" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E50">
         <v>2130</v>
@@ -2132,12 +2280,15 @@
         <v>79</v>
       </c>
       <c r="G50">
+        <v>7</v>
+      </c>
+      <c r="H50">
         <v>15.8</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -2146,7 +2297,7 @@
         <v>2472</v>
       </c>
       <c r="D51" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E51">
         <v>2670</v>
@@ -2155,12 +2306,15 @@
         <v>79</v>
       </c>
       <c r="G51">
+        <v>4</v>
+      </c>
+      <c r="H51">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B52">
         <v>6</v>
@@ -2169,7 +2323,7 @@
         <v>2834</v>
       </c>
       <c r="D52" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E52">
         <v>2595</v>
@@ -2178,12 +2332,15 @@
         <v>79</v>
       </c>
       <c r="G52">
+        <v>4</v>
+      </c>
+      <c r="H52">
         <v>12.2</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B53">
         <v>6</v>
@@ -2192,7 +2349,7 @@
         <v>2834</v>
       </c>
       <c r="D53" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E53">
         <v>2700</v>
@@ -2201,12 +2358,15 @@
         <v>79</v>
       </c>
       <c r="G53">
+        <v>4</v>
+      </c>
+      <c r="H53">
         <v>11.3</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -2215,7 +2375,7 @@
         <v>2474</v>
       </c>
       <c r="D54" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E54">
         <v>2556</v>
@@ -2224,12 +2384,15 @@
         <v>79</v>
       </c>
       <c r="G54">
+        <v>4</v>
+      </c>
+      <c r="H54">
         <v>14.2</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -2238,7 +2401,7 @@
         <v>1605</v>
       </c>
       <c r="D55" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E55">
         <v>2144</v>
@@ -2247,12 +2410,15 @@
         <v>80</v>
       </c>
       <c r="G55">
+        <v>3</v>
+      </c>
+      <c r="H55">
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -2261,7 +2427,7 @@
         <v>1458</v>
       </c>
       <c r="D56" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E56">
         <v>1968</v>
@@ -2270,12 +2436,15 @@
         <v>80</v>
       </c>
       <c r="G56">
+        <v>4</v>
+      </c>
+      <c r="H56">
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57">
         <v>4</v>
@@ -2284,7 +2453,7 @@
         <v>1605</v>
       </c>
       <c r="D57" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E57">
         <v>2120</v>
@@ -2293,12 +2462,15 @@
         <v>80</v>
       </c>
       <c r="G57">
+        <v>3</v>
+      </c>
+      <c r="H57">
         <v>13.6</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B58">
         <v>4</v>
@@ -2307,7 +2479,7 @@
         <v>1409</v>
       </c>
       <c r="D58" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E58">
         <v>2019</v>
@@ -2316,12 +2488,15 @@
         <v>80</v>
       </c>
       <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="H58">
         <v>15.8</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>4</v>
@@ -2330,7 +2505,7 @@
         <v>2474</v>
       </c>
       <c r="D59" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E59">
         <v>2678</v>
@@ -2339,12 +2514,15 @@
         <v>80</v>
       </c>
       <c r="G59">
+        <v>3</v>
+      </c>
+      <c r="H59">
         <v>11.9</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60">
         <v>4</v>
@@ -2353,7 +2531,7 @@
         <v>2294</v>
       </c>
       <c r="D60" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E60">
         <v>2870</v>
@@ -2362,12 +2540,15 @@
         <v>80</v>
       </c>
       <c r="G60">
+        <v>4</v>
+      </c>
+      <c r="H60">
         <v>11.2</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61">
         <v>4</v>
@@ -2376,7 +2557,7 @@
         <v>2474</v>
       </c>
       <c r="D61" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E61">
         <v>3003</v>
@@ -2385,12 +2566,15 @@
         <v>80</v>
       </c>
       <c r="G61">
+        <v>4</v>
+      </c>
+      <c r="H61">
         <v>10.3</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62">
         <v>6</v>
@@ -2399,7 +2583,7 @@
         <v>3687</v>
       </c>
       <c r="D62" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E62">
         <v>3381</v>
@@ -2408,12 +2592,15 @@
         <v>80</v>
       </c>
       <c r="G62">
+        <v>4</v>
+      </c>
+      <c r="H62">
         <v>8.1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63">
         <v>4</v>
@@ -2422,7 +2609,7 @@
         <v>1589</v>
       </c>
       <c r="D63" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E63">
         <v>2188</v>
@@ -2431,12 +2618,15 @@
         <v>80</v>
       </c>
       <c r="G63">
+        <v>4</v>
+      </c>
+      <c r="H63">
         <v>14.5</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B64">
         <v>4</v>
@@ -2445,7 +2635,7 @@
         <v>2195</v>
       </c>
       <c r="D64" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E64">
         <v>2711</v>
@@ -2454,12 +2644,15 @@
         <v>80</v>
       </c>
       <c r="G64">
+        <v>4</v>
+      </c>
+      <c r="H64">
         <v>12.6</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B65">
         <v>4</v>
@@ -2468,7 +2661,7 @@
         <v>1966</v>
       </c>
       <c r="D65" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E65">
         <v>2542</v>
@@ -2477,12 +2670,15 @@
         <v>80</v>
       </c>
       <c r="G65">
+        <v>4</v>
+      </c>
+      <c r="H65">
         <v>13.3</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
       <c r="B66">
         <v>4</v>
@@ -2491,7 +2687,7 @@
         <v>1950</v>
       </c>
       <c r="D66" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E66">
         <v>2434</v>
@@ -2500,12 +2696,15 @@
         <v>80</v>
       </c>
       <c r="G66">
+        <v>3</v>
+      </c>
+      <c r="H66">
         <v>15.7</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B67">
         <v>4</v>
@@ -2514,7 +2713,7 @@
         <v>1769</v>
       </c>
       <c r="D67" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E67">
         <v>2265</v>
@@ -2523,12 +2722,15 @@
         <v>80</v>
       </c>
       <c r="G67">
+        <v>4</v>
+      </c>
+      <c r="H67">
         <v>13.6</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B68">
         <v>4</v>
@@ -2537,7 +2739,7 @@
         <v>1409</v>
       </c>
       <c r="D68" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E68">
         <v>2110</v>
@@ -2546,12 +2748,15 @@
         <v>80</v>
       </c>
       <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="H68">
         <v>19.8</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -2560,7 +2765,7 @@
         <v>2256</v>
       </c>
       <c r="D69" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E69">
         <v>2800</v>
@@ -2569,12 +2774,15 @@
         <v>80</v>
       </c>
       <c r="G69">
+        <v>4</v>
+      </c>
+      <c r="H69">
         <v>11.8</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -2583,7 +2791,7 @@
         <v>1392</v>
       </c>
       <c r="D70" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E70">
         <v>2110</v>
@@ -2592,12 +2800,15 @@
         <v>80</v>
       </c>
       <c r="G70">
+        <v>4</v>
+      </c>
+      <c r="H70">
         <v>17.34</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B71">
         <v>4</v>
@@ -2606,7 +2817,7 @@
         <v>1474</v>
       </c>
       <c r="D71" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E71">
         <v>2085</v>
@@ -2615,12 +2826,15 @@
         <v>80</v>
       </c>
       <c r="G71">
+        <v>3</v>
+      </c>
+      <c r="H71">
         <v>18.8</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B72">
         <v>4</v>
@@ -2629,7 +2843,7 @@
         <v>1474</v>
       </c>
       <c r="D72" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E72">
         <v>2335</v>
@@ -2638,12 +2852,15 @@
         <v>80</v>
       </c>
       <c r="G72">
+        <v>6</v>
+      </c>
+      <c r="H72">
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B73">
         <v>5</v>
@@ -2652,7 +2869,7 @@
         <v>1982</v>
       </c>
       <c r="D73" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E73">
         <v>2950</v>
@@ -2661,12 +2878,15 @@
         <v>80</v>
       </c>
       <c r="G73">
+        <v>4</v>
+      </c>
+      <c r="H73">
         <v>15.4</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B74">
         <v>4</v>
@@ -2675,7 +2895,7 @@
         <v>2392</v>
       </c>
       <c r="D74" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E74">
         <v>3250</v>
@@ -2684,12 +2904,15 @@
         <v>80</v>
       </c>
       <c r="G74">
+        <v>4</v>
+      </c>
+      <c r="H74">
         <v>12.7</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B75">
         <v>4</v>
@@ -2698,7 +2921,7 @@
         <v>1491</v>
       </c>
       <c r="D75" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E75">
         <v>1850</v>
@@ -2707,12 +2930,15 @@
         <v>80</v>
       </c>
       <c r="G75">
+        <v>4</v>
+      </c>
+      <c r="H75">
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B76">
         <v>4</v>
@@ -2721,7 +2947,7 @@
         <v>1392</v>
       </c>
       <c r="D76" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E76">
         <v>1835</v>
@@ -2730,12 +2956,15 @@
         <v>80</v>
       </c>
       <c r="G76">
+        <v>3</v>
+      </c>
+      <c r="H76">
         <v>17.3</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B77">
         <v>4</v>
@@ -2744,7 +2973,7 @@
         <v>1589</v>
       </c>
       <c r="D77" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E77">
         <v>2145</v>
@@ -2753,12 +2982,15 @@
         <v>80</v>
       </c>
       <c r="G77">
+        <v>4</v>
+      </c>
+      <c r="H77">
         <v>14.3</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B78">
         <v>4</v>
@@ -2767,7 +2999,7 @@
         <v>1458</v>
       </c>
       <c r="D78" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E78">
         <v>1845</v>
@@ -2776,12 +3008,15 @@
         <v>80</v>
       </c>
       <c r="G78">
+        <v>3</v>
+      </c>
+      <c r="H78">
         <v>12.6</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B79">
         <v>6</v>
@@ -2790,7 +3025,7 @@
         <v>2753</v>
       </c>
       <c r="D79" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E79">
         <v>2910</v>
@@ -2799,12 +3034,15 @@
         <v>80</v>
       </c>
       <c r="G79">
+        <v>3</v>
+      </c>
+      <c r="H79">
         <v>13.9</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B80">
         <v>3</v>
@@ -2813,7 +3051,7 @@
         <v>1147</v>
       </c>
       <c r="D80" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E80">
         <v>2420</v>
@@ -2822,12 +3060,15 @@
         <v>80</v>
       </c>
       <c r="G80">
+        <v>4</v>
+      </c>
+      <c r="H80">
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B81">
         <v>4</v>
@@ -2836,7 +3077,7 @@
         <v>1999</v>
       </c>
       <c r="D81" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E81">
         <v>2500</v>
@@ -2845,12 +3086,15 @@
         <v>80</v>
       </c>
       <c r="G81">
+        <v>4</v>
+      </c>
+      <c r="H81">
         <v>14.8</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -2859,7 +3103,7 @@
         <v>2294</v>
       </c>
       <c r="D82" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E82">
         <v>2905</v>
@@ -2868,12 +3112,15 @@
         <v>80</v>
       </c>
       <c r="G82">
+        <v>4</v>
+      </c>
+      <c r="H82">
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B83">
         <v>4</v>
@@ -2882,7 +3129,7 @@
         <v>1753</v>
       </c>
       <c r="D83" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E83">
         <v>2290</v>
@@ -2891,12 +3138,15 @@
         <v>80</v>
       </c>
       <c r="G83">
+        <v>4</v>
+      </c>
+      <c r="H83">
         <v>13.7</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B84">
         <v>4</v>
@@ -2905,7 +3155,7 @@
         <v>2212</v>
       </c>
       <c r="D84" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E84">
         <v>2490</v>
@@ -2914,12 +3164,15 @@
         <v>81</v>
       </c>
       <c r="G84">
+        <v>4</v>
+      </c>
+      <c r="H84">
         <v>11.5</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B85">
         <v>4</v>
@@ -2928,7 +3181,7 @@
         <v>2474</v>
       </c>
       <c r="D85" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E85">
         <v>2635</v>
@@ -2937,12 +3190,15 @@
         <v>81</v>
       </c>
       <c r="G85">
+        <v>4</v>
+      </c>
+      <c r="H85">
         <v>11.3</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>177</v>
       </c>
       <c r="B86">
         <v>4</v>
@@ -2951,7 +3207,7 @@
         <v>2556</v>
       </c>
       <c r="D86" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E86">
         <v>2620</v>
@@ -2960,12 +3216,15 @@
         <v>81</v>
       </c>
       <c r="G86">
+        <v>6</v>
+      </c>
+      <c r="H86">
         <v>10.9</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B87">
         <v>6</v>
@@ -2974,7 +3233,7 @@
         <v>2834</v>
       </c>
       <c r="D87" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E87">
         <v>2725</v>
@@ -2983,12 +3242,15 @@
         <v>81</v>
       </c>
       <c r="G87">
+        <v>3</v>
+      </c>
+      <c r="H87">
         <v>9.9</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B88">
         <v>4</v>
@@ -2997,7 +3259,7 @@
         <v>2195</v>
       </c>
       <c r="D88" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E88">
         <v>2385</v>
@@ -3006,12 +3268,15 @@
         <v>81</v>
       </c>
       <c r="G88">
+        <v>4</v>
+      </c>
+      <c r="H88">
         <v>12.7</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B89">
         <v>4</v>
@@ -3020,7 +3285,7 @@
         <v>1294</v>
       </c>
       <c r="D89" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E89">
         <v>1755</v>
@@ -3029,12 +3294,15 @@
         <v>81</v>
       </c>
       <c r="G89">
+        <v>3</v>
+      </c>
+      <c r="H89">
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B90">
         <v>4</v>
@@ -3043,7 +3311,7 @@
         <v>1409</v>
       </c>
       <c r="D90" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E90">
         <v>1875</v>
@@ -3052,12 +3320,15 @@
         <v>81</v>
       </c>
       <c r="G90">
+        <v>3</v>
+      </c>
+      <c r="H90">
         <v>16.5</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B91">
         <v>4</v>
@@ -3066,7 +3337,7 @@
         <v>1327</v>
       </c>
       <c r="D91" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E91">
         <v>1760</v>
@@ -3075,127 +3346,145 @@
         <v>81</v>
       </c>
       <c r="G91">
+        <v>4</v>
+      </c>
+      <c r="H91">
         <v>14.9</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B92">
         <v>4</v>
       </c>
       <c r="C92">
-        <v>1589</v>
+        <v>1392</v>
       </c>
       <c r="D92" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="E92">
-        <v>2065</v>
+        <v>1975</v>
       </c>
       <c r="F92">
         <v>81</v>
       </c>
       <c r="G92">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H92">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B93">
         <v>4</v>
       </c>
       <c r="C93">
-        <v>1392</v>
+        <v>1458</v>
       </c>
       <c r="D93" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="E93">
-        <v>1975</v>
+        <v>2050</v>
       </c>
       <c r="F93">
         <v>81</v>
       </c>
       <c r="G93">
-        <v>15.7</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H93">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B94">
         <v>4</v>
       </c>
       <c r="C94">
-        <v>1458</v>
+        <v>1491</v>
       </c>
       <c r="D94" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E94">
-        <v>2050</v>
+        <v>1985</v>
       </c>
       <c r="F94">
         <v>81</v>
       </c>
       <c r="G94">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H94">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B95">
         <v>4</v>
       </c>
       <c r="C95">
-        <v>1491</v>
+        <v>1720</v>
       </c>
       <c r="D95" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E95">
-        <v>1985</v>
+        <v>2215</v>
       </c>
       <c r="F95">
         <v>81</v>
       </c>
       <c r="G95">
-        <v>14.4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H95">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B96">
         <v>4</v>
       </c>
       <c r="C96">
-        <v>1720</v>
+        <v>1605</v>
       </c>
       <c r="D96" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="E96">
-        <v>2215</v>
+        <v>2045</v>
       </c>
       <c r="F96">
         <v>81</v>
       </c>
       <c r="G96">
-        <v>14.7</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H96">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B97">
         <v>4</v>
@@ -3204,366 +3493,414 @@
         <v>1605</v>
       </c>
       <c r="D97" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E97">
-        <v>2045</v>
+        <v>2380</v>
       </c>
       <c r="F97">
         <v>81</v>
       </c>
       <c r="G97">
-        <v>14.6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H97">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B98">
         <v>4</v>
       </c>
       <c r="C98">
-        <v>1605</v>
+        <v>1720</v>
       </c>
       <c r="D98" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="E98">
-        <v>2380</v>
+        <v>2190</v>
       </c>
       <c r="F98">
         <v>81</v>
       </c>
       <c r="G98">
-        <v>12.7</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H98">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B99">
         <v>4</v>
       </c>
       <c r="C99">
-        <v>1720</v>
+        <v>1638</v>
       </c>
       <c r="D99" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="E99">
-        <v>2190</v>
+        <v>2320</v>
       </c>
       <c r="F99">
         <v>81</v>
       </c>
       <c r="G99">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H99">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B100">
         <v>4</v>
       </c>
       <c r="C100">
-        <v>1638</v>
+        <v>1753</v>
       </c>
       <c r="D100" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="E100">
-        <v>2320</v>
+        <v>2210</v>
       </c>
       <c r="F100">
         <v>81</v>
       </c>
       <c r="G100">
-        <v>14.6</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H100">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="B101">
         <v>4</v>
       </c>
       <c r="C101">
-        <v>1753</v>
+        <v>1769</v>
       </c>
       <c r="D101" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E101">
-        <v>2210</v>
+        <v>2350</v>
       </c>
       <c r="F101">
         <v>81</v>
       </c>
       <c r="G101">
-        <v>14.3</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H101">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="B102">
         <v>4</v>
       </c>
       <c r="C102">
-        <v>1769</v>
+        <v>1950</v>
       </c>
       <c r="D102" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E102">
-        <v>2350</v>
+        <v>2615</v>
       </c>
       <c r="F102">
         <v>81</v>
       </c>
       <c r="G102">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H102">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="B103">
         <v>4</v>
       </c>
       <c r="C103">
-        <v>1950</v>
+        <v>1966</v>
       </c>
       <c r="D103" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E103">
-        <v>2615</v>
+        <v>2635</v>
       </c>
       <c r="F103">
         <v>81</v>
       </c>
       <c r="G103">
-        <v>13.9</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H103">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="B104">
         <v>4</v>
       </c>
       <c r="C104">
-        <v>1966</v>
+        <v>2310</v>
       </c>
       <c r="D104" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="E104">
-        <v>2635</v>
+        <v>3230</v>
       </c>
       <c r="F104">
         <v>81</v>
       </c>
       <c r="G104">
-        <v>13.4</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H104">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B105">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C105">
-        <v>2310</v>
+        <v>2376</v>
       </c>
       <c r="D105" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E105">
-        <v>3230</v>
+        <v>3160</v>
       </c>
       <c r="F105">
         <v>81</v>
       </c>
       <c r="G105">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H105">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B106">
         <v>6</v>
       </c>
       <c r="C106">
-        <v>2376</v>
+        <v>2753</v>
       </c>
       <c r="D106" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="E106">
-        <v>3160</v>
+        <v>2900</v>
       </c>
       <c r="F106">
         <v>81</v>
       </c>
       <c r="G106">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H106">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B107">
         <v>6</v>
       </c>
       <c r="C107">
-        <v>2753</v>
+        <v>2392</v>
       </c>
       <c r="D107" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E107">
-        <v>2900</v>
+        <v>2930</v>
       </c>
       <c r="F107">
         <v>81</v>
       </c>
       <c r="G107">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H107">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B108">
         <v>6</v>
       </c>
       <c r="C108">
-        <v>2392</v>
+        <v>3785</v>
       </c>
       <c r="D108" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="E108">
-        <v>2930</v>
+        <v>3415</v>
       </c>
       <c r="F108">
         <v>81</v>
       </c>
       <c r="G108">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H108">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B109">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C109">
-        <v>3785</v>
+        <v>5735</v>
       </c>
       <c r="D109" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="E109">
-        <v>3415</v>
+        <v>3725</v>
       </c>
       <c r="F109">
         <v>81</v>
       </c>
       <c r="G109">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H109">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B110">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C110">
-        <v>5735</v>
+        <v>3277</v>
       </c>
       <c r="D110" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E110">
-        <v>3725</v>
+        <v>3060</v>
       </c>
       <c r="F110">
         <v>81</v>
       </c>
       <c r="G110">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H110">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B111">
         <v>6</v>
       </c>
       <c r="C111">
-        <v>3277</v>
+        <v>3687</v>
       </c>
       <c r="D111" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="E111">
-        <v>3060</v>
+        <v>3465</v>
       </c>
       <c r="F111">
         <v>81</v>
       </c>
       <c r="G111">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H111">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B112">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C112">
-        <v>3687</v>
+        <v>1835</v>
       </c>
       <c r="D112" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="E112">
-        <v>3465</v>
+        <v>2605</v>
       </c>
       <c r="F112">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G112">
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H112">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>178</v>
       </c>
       <c r="B113">
         <v>4</v>
@@ -3572,21 +3909,24 @@
         <v>1835</v>
       </c>
       <c r="D113" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E113">
-        <v>2605</v>
+        <v>2640</v>
       </c>
       <c r="F113">
         <v>82</v>
       </c>
       <c r="G113">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="H113">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B114">
         <v>4</v>
@@ -3595,21 +3935,24 @@
         <v>1835</v>
       </c>
       <c r="D114" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E114">
-        <v>2640</v>
+        <v>2395</v>
       </c>
       <c r="F114">
         <v>82</v>
       </c>
       <c r="G114">
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H114">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>115</v>
+        <v>176</v>
       </c>
       <c r="B115">
         <v>4</v>
@@ -3618,159 +3961,180 @@
         <v>1835</v>
       </c>
       <c r="D115" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="E115">
-        <v>2395</v>
+        <v>2575</v>
       </c>
       <c r="F115">
         <v>82</v>
       </c>
       <c r="G115">
-        <v>14.4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H115">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B116">
         <v>4</v>
       </c>
       <c r="C116">
-        <v>1835</v>
+        <v>2212</v>
       </c>
       <c r="D116" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="E116">
-        <v>2575</v>
+        <v>2525</v>
       </c>
       <c r="F116">
         <v>82</v>
       </c>
       <c r="G116">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H116">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="B117">
         <v>4</v>
       </c>
       <c r="C117">
-        <v>2212</v>
+        <v>2474</v>
       </c>
       <c r="D117" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="E117">
-        <v>2525</v>
+        <v>2735</v>
       </c>
       <c r="F117">
         <v>82</v>
       </c>
       <c r="G117">
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H117">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="B118">
         <v>4</v>
       </c>
       <c r="C118">
-        <v>2474</v>
+        <v>2294</v>
       </c>
       <c r="D118" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E118">
-        <v>2735</v>
+        <v>2865</v>
       </c>
       <c r="F118">
         <v>82</v>
       </c>
       <c r="G118">
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H118">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B119">
         <v>4</v>
       </c>
       <c r="C119">
-        <v>2294</v>
+        <v>2474</v>
       </c>
       <c r="D119" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E119">
-        <v>2865</v>
+        <v>3035</v>
       </c>
       <c r="F119">
         <v>82</v>
       </c>
       <c r="G119">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H119">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B120">
         <v>4</v>
       </c>
       <c r="C120">
-        <v>2474</v>
+        <v>1720</v>
       </c>
       <c r="D120" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E120">
-        <v>3035</v>
+        <v>1980</v>
       </c>
       <c r="F120">
         <v>82</v>
       </c>
       <c r="G120">
-        <v>9.6999999999999993</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H120">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B121">
         <v>4</v>
       </c>
       <c r="C121">
-        <v>1720</v>
+        <v>1491</v>
       </c>
       <c r="D121" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E121">
-        <v>1980</v>
+        <v>2025</v>
       </c>
       <c r="F121">
         <v>82</v>
       </c>
       <c r="G121">
-        <v>15.3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H121">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B122">
         <v>4</v>
@@ -3779,53 +4143,59 @@
         <v>1491</v>
       </c>
       <c r="D122" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E122">
-        <v>2025</v>
+        <v>1970</v>
       </c>
       <c r="F122">
         <v>82</v>
       </c>
       <c r="G122">
-        <v>15.7</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H122">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B123">
         <v>4</v>
       </c>
       <c r="C123">
-        <v>1491</v>
+        <v>1720</v>
       </c>
       <c r="D123" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E123">
-        <v>1970</v>
+        <v>2125</v>
       </c>
       <c r="F123">
         <v>82</v>
       </c>
       <c r="G123">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H123">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B124">
         <v>4</v>
       </c>
       <c r="C124">
-        <v>1720</v>
+        <v>1605</v>
       </c>
       <c r="D124" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="E124">
         <v>2125</v>
@@ -3834,104 +4204,119 @@
         <v>82</v>
       </c>
       <c r="G124">
-        <v>16.100000000000001</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="H124">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B125">
         <v>4</v>
       </c>
       <c r="C125">
-        <v>1605</v>
+        <v>1966</v>
       </c>
       <c r="D125" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E125">
-        <v>2125</v>
+        <v>2160</v>
       </c>
       <c r="F125">
         <v>82</v>
       </c>
       <c r="G125">
+        <v>4</v>
+      </c>
+      <c r="H125">
         <v>15.3</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="B126">
         <v>4</v>
       </c>
       <c r="C126">
-        <v>1966</v>
+        <v>1753</v>
       </c>
       <c r="D126" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E126">
-        <v>2160</v>
+        <v>2205</v>
       </c>
       <c r="F126">
         <v>82</v>
       </c>
       <c r="G126">
+        <v>4</v>
+      </c>
+      <c r="H126">
         <v>15.3</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="B127">
         <v>4</v>
       </c>
       <c r="C127">
-        <v>1753</v>
+        <v>1769</v>
       </c>
       <c r="D127" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="E127">
-        <v>2205</v>
+        <v>2245</v>
       </c>
       <c r="F127">
         <v>82</v>
       </c>
       <c r="G127">
-        <v>15.3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H127">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="B128">
         <v>4</v>
       </c>
       <c r="C128">
-        <v>1769</v>
+        <v>1491</v>
       </c>
       <c r="D128" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E128">
-        <v>2245</v>
+        <v>1965</v>
       </c>
       <c r="F128">
         <v>82</v>
       </c>
       <c r="G128">
-        <v>14.4</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H128">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B129">
         <v>4</v>
@@ -3940,7 +4325,7 @@
         <v>1491</v>
       </c>
       <c r="D129" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E129">
         <v>1965</v>
@@ -3949,12 +4334,15 @@
         <v>82</v>
       </c>
       <c r="G129">
-        <v>16.100000000000001</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H129">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B130">
         <v>4</v>
@@ -3963,314 +4351,330 @@
         <v>1491</v>
       </c>
       <c r="D130" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E130">
-        <v>1965</v>
+        <v>1995</v>
       </c>
       <c r="F130">
         <v>82</v>
       </c>
       <c r="G130">
-        <v>13.6</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H130">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B131">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C131">
-        <v>1491</v>
+        <v>2966</v>
       </c>
       <c r="D131" t="s">
         <v>158</v>
       </c>
       <c r="E131">
-        <v>1995</v>
+        <v>2945</v>
       </c>
       <c r="F131">
         <v>82</v>
       </c>
       <c r="G131">
-        <v>16.100000000000001</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H131">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B132">
         <v>6</v>
       </c>
       <c r="C132">
-        <v>2966</v>
+        <v>4293</v>
       </c>
       <c r="D132" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E132">
-        <v>2945</v>
+        <v>3015</v>
       </c>
       <c r="F132">
         <v>82</v>
       </c>
       <c r="G132">
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H132">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B133">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C133">
-        <v>4293</v>
+        <v>2556</v>
       </c>
       <c r="D133" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="E133">
-        <v>3015</v>
+        <v>2585</v>
       </c>
       <c r="F133">
         <v>82</v>
       </c>
       <c r="G133">
-        <v>16.100000000000001</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H133">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B134">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C134">
-        <v>2556</v>
+        <v>3801</v>
       </c>
       <c r="D134" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="E134">
-        <v>2585</v>
+        <v>2835</v>
       </c>
       <c r="F134">
         <v>82</v>
       </c>
       <c r="G134">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H134">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B135">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C135">
-        <v>3801</v>
+        <v>2359</v>
       </c>
       <c r="D135" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E135">
-        <v>2835</v>
+        <v>2665</v>
       </c>
       <c r="F135">
         <v>82</v>
       </c>
       <c r="G135">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H135">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B136">
         <v>4</v>
       </c>
       <c r="C136">
-        <v>2359</v>
+        <v>2212</v>
       </c>
       <c r="D136" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="E136">
-        <v>2665</v>
+        <v>2370</v>
       </c>
       <c r="F136">
         <v>82</v>
       </c>
       <c r="G136">
-        <v>13.6</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H136">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B137">
         <v>4</v>
       </c>
       <c r="C137">
-        <v>2212</v>
+        <v>2474</v>
       </c>
       <c r="D137" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="E137">
-        <v>2370</v>
+        <v>2950</v>
       </c>
       <c r="F137">
         <v>82</v>
       </c>
       <c r="G137">
-        <v>15.3</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H137">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B138">
         <v>4</v>
       </c>
       <c r="C138">
-        <v>2474</v>
+        <v>2294</v>
       </c>
       <c r="D138" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="E138">
-        <v>2950</v>
+        <v>2790</v>
       </c>
       <c r="F138">
         <v>82</v>
       </c>
       <c r="G138">
+        <v>4</v>
+      </c>
+      <c r="H138">
         <v>11.4</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="B139">
         <v>4</v>
       </c>
       <c r="C139">
-        <v>2294</v>
+        <v>1589</v>
       </c>
       <c r="D139" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E139">
-        <v>2790</v>
+        <v>2130</v>
       </c>
       <c r="F139">
         <v>82</v>
       </c>
       <c r="G139">
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="H139">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B140">
         <v>4</v>
       </c>
       <c r="C140">
-        <v>1589</v>
+        <v>2212</v>
       </c>
       <c r="D140" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="E140">
-        <v>2130</v>
+        <v>2295</v>
       </c>
       <c r="F140">
         <v>82</v>
       </c>
       <c r="G140">
-        <v>18.7</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="H140">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B141">
         <v>4</v>
       </c>
       <c r="C141">
-        <v>2212</v>
+        <v>1966</v>
       </c>
       <c r="D141" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="E141">
-        <v>2295</v>
+        <v>2625</v>
       </c>
       <c r="F141">
         <v>82</v>
       </c>
       <c r="G141">
-        <v>13.6</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="H141">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B142">
         <v>4</v>
       </c>
       <c r="C142">
-        <v>1966</v>
+        <v>1950</v>
       </c>
       <c r="D142" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E142">
-        <v>2625</v>
+        <v>2720</v>
       </c>
       <c r="F142">
         <v>82</v>
       </c>
       <c r="G142">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>140</v>
-      </c>
-      <c r="B143">
-        <v>4</v>
-      </c>
-      <c r="C143">
-        <v>1950</v>
-      </c>
-      <c r="D143" t="s">
-        <v>179</v>
-      </c>
-      <c r="E143">
-        <v>2720</v>
-      </c>
-      <c r="F143">
-        <v>82</v>
-      </c>
-      <c r="G143">
+        <v>7</v>
+      </c>
+      <c r="H142">
         <v>13.1</v>
       </c>
     </row>

</xml_diff>